<commit_message>
Add zip IN + Modify region quota
</commit_message>
<xml_diff>
--- a/questionnaires/quotas.xlsx
+++ b/questionnaires/quotas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CE7E90-95B0-C94A-88DE-5050B6D8827B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554D6FD7-E7E9-5541-9BB9-A96CD0FBA67A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2820" yWindow="-15620" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotas_US" sheetId="2" r:id="rId1"/>
@@ -412,13 +412,7 @@
     <t>Central Zonal Council</t>
   </si>
   <si>
-    <t>Eastern Zonal Council</t>
-  </si>
-  <si>
     <t>Western Zonal Council</t>
-  </si>
-  <si>
-    <t>Rest (North Eastern)</t>
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Zonal_Council</t>
@@ -977,6 +971,12 @@
   </si>
   <si>
     <t>https://www.canadapost-postescanada.ca/cpc/en/support/articles/addressing-guidelines/postal-codes.page?</t>
+  </si>
+  <si>
+    <t>Southern Zonal Council also includes: Andaman and Nicobar Islands, Lakshadweep</t>
+  </si>
+  <si>
+    <t>Eastern Zonal Council + North Eastern</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1112,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1172,6 +1172,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1960,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -2203,7 +2204,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:11" ht="44" thickBot="1">
+    <row r="14" spans="1:11" ht="72" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -2217,15 +2218,16 @@
         <v>119</v>
       </c>
       <c r="E14" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>122</v>
-      </c>
+      <c r="G14" s="29"/>
       <c r="H14" s="25"/>
+      <c r="K14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
@@ -2241,16 +2243,13 @@
         <v>0.26537793566411777</v>
       </c>
       <c r="E15" s="21">
-        <v>0.22558586499486741</v>
+        <v>0.26349328733071997</v>
       </c>
       <c r="F15" s="22">
         <v>0.13797875654055569</v>
       </c>
-      <c r="G15">
-        <v>3.7907422335852557E-2</v>
-      </c>
-      <c r="H15" s="17">
-        <f>SUM(B15:G15)</f>
+      <c r="G15" s="17">
+        <f>SUM(B15:F15)</f>
         <v>0.99999999999999989</v>
       </c>
     </row>
@@ -2272,22 +2271,18 @@
       </c>
       <c r="E16" s="10">
         <f t="shared" si="2"/>
-        <v>451</v>
+        <v>527</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="2"/>
         <v>276</v>
       </c>
-      <c r="G16" s="10">
-        <f t="shared" si="2"/>
-        <v>76</v>
-      </c>
-      <c r="H16" s="3">
-        <f>SUM(B16:G16)</f>
+      <c r="G16" s="3">
+        <f>SUM(B16:F16)</f>
         <v>2000</v>
       </c>
       <c r="K16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" thickBot="1">
@@ -2308,22 +2303,18 @@
       </c>
       <c r="E17" s="2">
         <f t="shared" si="3"/>
-        <v>496</v>
+        <v>580</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="3"/>
         <v>304</v>
       </c>
-      <c r="G17" s="2">
-        <f t="shared" si="3"/>
-        <v>83</v>
-      </c>
-      <c r="H17" s="3">
-        <f>SUM(B17:G17)</f>
-        <v>2200</v>
+      <c r="G17" s="3">
+        <f>SUM(B17:F17)</f>
+        <v>2201</v>
       </c>
       <c r="K17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -2334,6 +2325,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
+      <c r="F18" s="33"/>
       <c r="H18" s="25"/>
     </row>
     <row r="19" spans="1:12">
@@ -2356,21 +2348,21 @@
       <c r="G20" s="28"/>
       <c r="H20" s="25"/>
       <c r="K20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="L20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -2465,25 +2457,25 @@
     </row>
     <row r="28" spans="1:12" ht="30" thickBot="1">
       <c r="A28" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B28" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="D28" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="E28" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="F28" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="G28" s="29" t="s">
         <v>149</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="G28" s="29" t="s">
-        <v>151</v>
       </c>
       <c r="H28" s="25"/>
     </row>
@@ -2840,28 +2832,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="E14" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="F14" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="G14" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" t="s">
         <v>163</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="K14" t="s">
         <v>164</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="J14" t="s">
-        <v>165</v>
-      </c>
-      <c r="K14" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -2888,10 +2880,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -2923,10 +2915,10 @@
         <v>2001</v>
       </c>
       <c r="J16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -2958,10 +2950,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2973,15 +2965,15 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
       <c r="J18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="K19" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" thickBot="1"/>
@@ -3014,10 +3006,10 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="16" thickBot="1">
@@ -3038,10 +3030,10 @@
       </c>
       <c r="E25" s="20"/>
       <c r="F25" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G25" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="44" thickBot="1">
@@ -3273,13 +3265,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>48</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>108</v>
@@ -3288,7 +3280,7 @@
         <v>114</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16" thickBot="1">
@@ -3315,10 +3307,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -3350,10 +3342,10 @@
         <v>2000</v>
       </c>
       <c r="J16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -3385,10 +3377,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -3400,10 +3392,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
       <c r="J18" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1"/>
@@ -3436,10 +3428,10 @@
       </c>
       <c r="E23" s="7"/>
       <c r="F23" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16" thickBot="1">
@@ -3460,13 +3452,13 @@
       </c>
       <c r="E24" s="20"/>
       <c r="F24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="44" thickBot="1">
@@ -3697,22 +3689,22 @@
         <v>13</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>48</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="16" thickBot="1">
@@ -3739,10 +3731,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J14" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -3774,10 +3766,10 @@
         <v>2000</v>
       </c>
       <c r="I15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J15" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -3844,10 +3836,10 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="16" thickBot="1">
@@ -3884,13 +3876,13 @@
         <v>2200</v>
       </c>
       <c r="G22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -3898,10 +3890,10 @@
         <v>30</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -3909,10 +3901,10 @@
     </row>
     <row r="24" spans="1:9">
       <c r="G24" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -3920,10 +3912,10 @@
     </row>
     <row r="25" spans="1:9">
       <c r="G25" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I25">
         <v>1</v>
@@ -3931,10 +3923,10 @@
     </row>
     <row r="26" spans="1:9">
       <c r="G26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H26" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -3942,7 +3934,7 @@
     </row>
     <row r="27" spans="1:9">
       <c r="G27" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -3950,7 +3942,7 @@
     </row>
     <row r="28" spans="1:9">
       <c r="G28" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -3958,10 +3950,10 @@
     </row>
     <row r="29" spans="1:9">
       <c r="G29" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H29" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -3969,10 +3961,10 @@
     </row>
     <row r="30" spans="1:9">
       <c r="G30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H30" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -3980,10 +3972,10 @@
     </row>
     <row r="31" spans="1:9">
       <c r="G31" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H31" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -3998,7 +3990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -4199,7 +4191,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>108</v>
@@ -4211,10 +4203,10 @@
         <v>47</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="16" thickBot="1">
@@ -4299,10 +4291,10 @@
         <v>2200</v>
       </c>
       <c r="I17" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J17" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -4524,10 +4516,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>108</v>
@@ -4539,13 +4531,13 @@
         <v>47</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -4572,10 +4564,10 @@
         <v>1.0000000000000011</v>
       </c>
       <c r="I15" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" thickBot="1">
@@ -4610,7 +4602,7 @@
         <v>108</v>
       </c>
       <c r="J16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" thickBot="1">
@@ -4645,7 +4637,7 @@
         <v>107</v>
       </c>
       <c r="J17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -4660,15 +4652,15 @@
         <v>47</v>
       </c>
       <c r="J18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="I19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -4881,25 +4873,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>112</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -4926,10 +4918,10 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" thickBot="1">
@@ -4961,10 +4953,10 @@
         <v>2000</v>
       </c>
       <c r="I16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" thickBot="1">
@@ -4999,7 +4991,7 @@
         <v>112</v>
       </c>
       <c r="J17" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5011,18 +5003,18 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
       <c r="I18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J18" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="I19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>
@@ -5232,28 +5224,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>248</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="E14" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="F14" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="G14" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" t="s">
         <v>253</v>
       </c>
-      <c r="F14" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="I14" t="s">
-        <v>255</v>
-      </c>
       <c r="J14" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -5280,7 +5272,7 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="I15" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" thickBot="1">
@@ -5312,10 +5304,10 @@
         <v>2000</v>
       </c>
       <c r="I16" s="29" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J16" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" thickBot="1">
@@ -5347,7 +5339,7 @@
         <v>2201</v>
       </c>
       <c r="I17" s="29" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5359,18 +5351,18 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
       <c r="I18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="I19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="16" thickBot="1"/>
@@ -5403,10 +5395,10 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G24" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16" thickBot="1">
@@ -5427,10 +5419,10 @@
       </c>
       <c r="E25" s="20"/>
       <c r="F25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G25" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="44" thickBot="1">
@@ -5451,12 +5443,12 @@
       </c>
       <c r="E26" s="20"/>
       <c r="G26" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="G27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -5672,22 +5664,22 @@
         <v>111</v>
       </c>
       <c r="D14" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>257</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>258</v>
-      </c>
       <c r="G14" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I14" t="s">
         <v>48</v>
       </c>
       <c r="J14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -5717,7 +5709,7 @@
         <v>111</v>
       </c>
       <c r="J15" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" thickBot="1">
@@ -5749,7 +5741,7 @@
         <v>2000</v>
       </c>
       <c r="I16" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" thickBot="1">
@@ -5781,7 +5773,7 @@
         <v>2201</v>
       </c>
       <c r="I17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -5793,18 +5785,18 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
       <c r="I18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="I19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="30" thickBot="1">
@@ -5868,10 +5860,10 @@
         <v>2200</v>
       </c>
       <c r="I23" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J23" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
   </sheetData>
@@ -6081,28 +6073,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="E14" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="F14" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="G14" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" s="29" t="s">
         <v>282</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="J14" s="29" t="s">
         <v>283</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="I14" s="29" t="s">
-        <v>284</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -6198,10 +6190,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="I19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -6898,13 +6890,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>47</v>
@@ -6913,13 +6905,13 @@
         <v>48</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J14" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -6946,10 +6938,10 @@
         <v>0.99999999999999933</v>
       </c>
       <c r="I15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="J15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="16" thickBot="1">
@@ -6981,10 +6973,10 @@
         <v>1999</v>
       </c>
       <c r="I16" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J16" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -7019,7 +7011,7 @@
         <v>47</v>
       </c>
       <c r="J17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -7034,18 +7026,18 @@
         <v>48</v>
       </c>
       <c r="J18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="I19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="K19" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -8424,10 +8416,10 @@
     </row>
     <row r="19" spans="1:11" ht="16">
       <c r="J19" t="s">
+        <v>234</v>
+      </c>
+      <c r="K19" s="32" t="s">
         <v>236</v>
-      </c>
-      <c r="K19" s="32" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" thickBot="1">
@@ -8438,10 +8430,10 @@
         <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="30" thickBot="1">
@@ -8483,10 +8475,10 @@
         <v>1999</v>
       </c>
       <c r="F22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="30" thickBot="1">
@@ -8510,10 +8502,10 @@
         <v>2200</v>
       </c>
       <c r="F23" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -8843,7 +8835,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="11"/>
       <c r="J17" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1">
@@ -8917,10 +8909,10 @@
         <v>85</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>51</v>
@@ -8987,7 +8979,7 @@
         <v>2200</v>
       </c>
       <c r="H28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -8999,7 +8991,7 @@
       <c r="D29" s="10"/>
       <c r="E29" s="10"/>
       <c r="H29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -9212,7 +9204,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>111</v>
@@ -9230,10 +9222,10 @@
         <v>114</v>
       </c>
       <c r="L13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M13" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" thickBot="1">
@@ -9264,7 +9256,7 @@
         <v>111</v>
       </c>
       <c r="M14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="16" thickBot="1">
@@ -9300,7 +9292,7 @@
         <v>112</v>
       </c>
       <c r="M15" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" thickBot="1">
@@ -9336,7 +9328,7 @@
         <v>113</v>
       </c>
       <c r="M16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -9356,10 +9348,10 @@
     </row>
     <row r="18" spans="1:13">
       <c r="L18" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="16" thickBot="1"/>
@@ -9733,22 +9725,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -9776,10 +9768,10 @@
       </c>
       <c r="H15" s="17"/>
       <c r="J15" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -9812,10 +9804,10 @@
       </c>
       <c r="H16" s="3"/>
       <c r="J16" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K16" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -9851,7 +9843,7 @@
         <v>47</v>
       </c>
       <c r="K17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -9863,10 +9855,10 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
       <c r="J18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -9874,15 +9866,15 @@
         <v>107</v>
       </c>
       <c r="K19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="J20" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" thickBot="1">
@@ -10158,7 +10150,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="J13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="30" thickBot="1">
@@ -10166,25 +10158,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="D14" s="18" t="s">
+      <c r="J14" t="s">
         <v>226</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="J14" t="s">
-        <v>228</v>
-      </c>
       <c r="K14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="30" thickBot="1">
@@ -10211,10 +10203,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K15" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="16" thickBot="1">
@@ -10246,10 +10238,10 @@
         <v>1999</v>
       </c>
       <c r="J16" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="30" thickBot="1">
@@ -10281,10 +10273,10 @@
         <v>2200</v>
       </c>
       <c r="J17" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K17" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -10296,7 +10288,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
       <c r="J18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" thickBot="1"/>
@@ -10305,13 +10297,13 @@
         <v>85</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>125</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="E21" s="12"/>
     </row>
@@ -10354,7 +10346,7 @@
         <v>2002</v>
       </c>
       <c r="H23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="44" thickBot="1">
@@ -10378,7 +10370,7 @@
         <v>2200</v>
       </c>
       <c r="H24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -10600,22 +10592,22 @@
         <v>13</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>47</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30" thickBot="1">
@@ -10642,10 +10634,10 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="J14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16" thickBot="1">
@@ -10680,7 +10672,7 @@
         <v>47</v>
       </c>
       <c r="J15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" thickBot="1">
@@ -10712,10 +10704,10 @@
         <v>2200</v>
       </c>
       <c r="I16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -10727,7 +10719,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="11"/>
       <c r="J17" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16" thickBot="1"/>
@@ -10736,10 +10728,10 @@
         <v>85</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>

</xml_diff>

<commit_message>
Add urban + zip MX
</commit_message>
<xml_diff>
--- a/questionnaires/quotas.xlsx
+++ b/questionnaires/quotas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554D6FD7-E7E9-5541-9BB9-A96CD0FBA67A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6268BF8-E7F7-0246-AD37-B5CA6F2A6692}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="-15620" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotas_US" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="312">
   <si>
     <t>IDF</t>
   </si>
@@ -977,6 +977,27 @@
   </si>
   <si>
     <t>Eastern Zonal Council + North Eastern</t>
+  </si>
+  <si>
+    <t>Semiurban</t>
+  </si>
+  <si>
+    <t>https://www.issea.gob.mx/Docs/Censo%20INEGI%202021/Censo2020_Principales_resultados_EUM.pdf</t>
+  </si>
+  <si>
+    <t>Source: (slide 19)</t>
+  </si>
+  <si>
+    <t>https://www.inee.edu.mx/wp-content/uploads/2019/03/CS02-2011.pdf</t>
+  </si>
+  <si>
+    <t>&gt;15k</t>
+  </si>
+  <si>
+    <t>&lt;2.5k</t>
+  </si>
+  <si>
+    <t>&lt;15k; &gt;2.5k</t>
   </si>
 </sst>
 </file>
@@ -1961,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4313,10 +4334,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -4662,6 +4683,122 @@
       <c r="J19" t="s">
         <v>276</v>
       </c>
+    </row>
+    <row r="21" spans="1:10" ht="16" thickBot="1">
+      <c r="A21" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" t="s">
+        <v>305</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1">
+      <c r="A22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="17">
+        <v>0.214</v>
+      </c>
+      <c r="C22">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="D22" s="17">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="E22" s="17">
+        <f>SUM(B22:D22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <f>ROUND(2000*B22,0)</f>
+        <v>428</v>
+      </c>
+      <c r="C23">
+        <f>ROUND(2000*C22,0)</f>
+        <v>298</v>
+      </c>
+      <c r="D23">
+        <f>ROUND(2000*D22,0)</f>
+        <v>1274</v>
+      </c>
+      <c r="E23">
+        <f>SUM(B23:D23)</f>
+        <v>2000</v>
+      </c>
+      <c r="F23" t="s">
+        <v>307</v>
+      </c>
+      <c r="G23" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24">
+        <f>ROUND(2200*B22,0)</f>
+        <v>471</v>
+      </c>
+      <c r="C24">
+        <f>ROUND(2200*C22,0)</f>
+        <v>328</v>
+      </c>
+      <c r="D24">
+        <f>ROUND(2200*D22,0)</f>
+        <v>1401</v>
+      </c>
+      <c r="E24">
+        <f>SUM(B24:D24)</f>
+        <v>2200</v>
+      </c>
+      <c r="F24" t="s">
+        <v>208</v>
+      </c>
+      <c r="G24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G25" t="s">
+        <v>214</v>
+      </c>
+      <c r="H25" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="G26" t="s">
+        <v>305</v>
+      </c>
+      <c r="H26" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="G27" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="D28" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5027,7 +5164,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:D26"/>
+      <selection activeCell="A23" sqref="A23:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -7049,8 +7186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8077,8 +8214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add zip for TR
</commit_message>
<xml_diff>
--- a/questionnaires/quotas.xlsx
+++ b/questionnaires/quotas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED85C35-37DB-D042-AA74-16D275298F3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14475" tabRatio="923" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="7" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotas_US" sheetId="2" r:id="rId1"/>
@@ -33,7 +34,7 @@
     <sheet name="quota_TR" sheetId="21" r:id="rId19"/>
     <sheet name="quota_UA" sheetId="22" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="314">
   <si>
     <t>IDF</t>
   </si>
@@ -998,11 +999,17 @@
   <si>
     <t>&lt;15k; &gt;2.5k</t>
   </si>
+  <si>
+    <t>https://biruni.tuik.gov.tr/medas/?kn=95&amp;locale=tr</t>
+  </si>
+  <si>
+    <t>ADNKS-GK137474-O29001 İbbs-Düzey1, İbbs-Düzey2, İl Ve İlçe Nüfusları / 2020 / İlçe Düzeyi / HEPSI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -1204,7 +1211,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1481,14 +1488,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -1977,29 +1984,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -2014,7 +2021,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -2036,7 +2043,7 @@
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2058,7 +2065,7 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -2099,7 +2106,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -2109,7 +2116,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="25"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -2131,7 +2138,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:11" ht="27" thickBot="1">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -2156,7 +2163,7 @@
       </c>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -2186,7 +2193,7 @@
       </c>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:11" ht="27" thickBot="1">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -2231,7 +2238,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:11" ht="65.25" thickBot="1">
+    <row r="14" spans="1:11" ht="72" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -2256,7 +2263,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -2280,7 +2287,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -2312,7 +2319,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="27" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -2381,7 +2388,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="27" thickBot="1">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>218</v>
       </c>
@@ -2397,7 +2404,7 @@
       <c r="G21" s="29"/>
       <c r="H21" s="25"/>
     </row>
-    <row r="22" spans="1:12" ht="27" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -2416,7 +2423,7 @@
       <c r="E22" s="21"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -2436,7 +2443,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:12" ht="27" thickBot="1">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -2482,7 +2489,7 @@
       <c r="E27" s="11"/>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:12" ht="27" thickBot="1">
+    <row r="28" spans="1:12" ht="30" thickBot="1">
       <c r="A28" s="9" t="s">
         <v>218</v>
       </c>
@@ -2506,7 +2513,7 @@
       </c>
       <c r="H28" s="25"/>
     </row>
-    <row r="29" spans="1:12" ht="27" thickBot="1">
+    <row r="29" spans="1:12" ht="30" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>10</v>
       </c>
@@ -2533,7 +2540,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>11</v>
       </c>
@@ -2566,7 +2573,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="27" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
@@ -2655,16 +2662,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -2678,7 +2685,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -2699,7 +2706,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2720,7 +2727,7 @@
         <v>0.99792841994678028</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27.75" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -2739,8 +2746,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="34"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -2761,7 +2768,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2785,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -2814,7 +2821,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -2854,7 +2861,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="27" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -2883,7 +2890,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -2913,7 +2920,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -2948,7 +2955,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -3003,8 +3010,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="23" spans="1:11" ht="27" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>85</v>
       </c>
@@ -3017,7 +3024,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="27" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -3039,7 +3046,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
@@ -3063,7 +3070,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39.75" thickBot="1">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>89</v>
       </c>
@@ -3088,16 +3095,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -3111,7 +3118,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -3132,7 +3139,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -3153,7 +3160,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -3172,8 +3179,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -3194,7 +3201,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -3218,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -3247,7 +3254,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -3287,7 +3294,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -3310,7 +3317,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -3340,7 +3347,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -3375,7 +3382,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -3425,8 +3432,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="22" spans="1:11" ht="27" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>85</v>
       </c>
@@ -3439,7 +3446,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
@@ -3461,7 +3468,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
@@ -3488,7 +3495,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39.75" thickBot="1">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -3512,16 +3519,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -3535,7 +3542,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -3556,7 +3563,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -3577,7 +3584,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -3596,8 +3603,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -3618,7 +3625,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -3642,7 +3649,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -3671,7 +3678,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -3711,7 +3718,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="27" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -3734,7 +3741,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -3764,7 +3771,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -3799,7 +3806,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="27" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -3837,7 +3844,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="13" t="s">
         <v>76</v>
       </c>
@@ -3848,7 +3855,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -3869,7 +3876,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -3886,7 +3893,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="27" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -4014,16 +4021,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -4037,7 +4044,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4058,7 +4065,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -4079,7 +4086,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="27" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -4098,8 +4105,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -4120,7 +4127,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4144,7 +4151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -4173,7 +4180,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -4213,7 +4220,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -4236,7 +4243,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -4260,7 +4267,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -4289,7 +4296,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -4339,16 +4346,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B22" sqref="B22:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -4362,7 +4369,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4383,7 +4390,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -4404,7 +4411,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -4423,8 +4430,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -4445,7 +4452,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4469,7 +4476,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -4498,7 +4505,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -4538,7 +4545,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -4567,7 +4574,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -4597,7 +4604,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -4632,7 +4639,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -4690,7 +4697,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="13" t="s">
         <v>76</v>
       </c>
@@ -4704,7 +4711,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -4722,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -4749,7 +4756,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="27" thickBot="1">
+    <row r="24" spans="1:10" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -4812,16 +4819,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -4835,7 +4842,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4856,7 +4863,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -4877,7 +4884,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -4896,8 +4903,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -4918,7 +4925,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4942,7 +4949,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -4971,7 +4978,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -5011,7 +5018,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -5037,7 +5044,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -5067,7 +5074,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -5102,7 +5109,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -5166,16 +5173,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -5189,7 +5196,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -5209,7 +5216,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5228,7 +5235,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -5247,8 +5254,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -5269,7 +5276,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5293,7 +5300,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -5322,7 +5329,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -5362,7 +5369,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -5391,7 +5398,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -5418,7 +5425,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -5453,7 +5460,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -5508,8 +5515,8 @@
         <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="23" spans="1:10" ht="27" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1"/>
+    <row r="23" spans="1:10" ht="30" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>85</v>
       </c>
@@ -5522,7 +5529,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
+    <row r="24" spans="1:10" ht="16" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -5544,7 +5551,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+    <row r="25" spans="1:10" ht="16" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
@@ -5568,7 +5575,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="39.75" thickBot="1">
+    <row r="26" spans="1:10" ht="44" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>89</v>
       </c>
@@ -5600,16 +5607,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="D23" sqref="A20:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -5623,7 +5630,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -5643,7 +5650,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5662,7 +5669,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -5681,8 +5688,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -5703,7 +5710,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5727,7 +5734,7 @@
         <v>0.99999999999999944</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -5756,7 +5763,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -5796,7 +5803,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -5825,7 +5832,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -5855,7 +5862,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -5887,7 +5894,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -5934,7 +5941,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="I19" t="s">
         <v>234</v>
       </c>
@@ -5942,7 +5949,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="27" thickBot="1">
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>85</v>
       </c>
@@ -5954,7 +5961,7 @@
       </c>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -5969,7 +5976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -5986,7 +5993,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="27" thickBot="1">
+    <row r="23" spans="1:10" ht="30" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -6015,16 +6022,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:J19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -6038,7 +6045,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6058,7 +6065,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -6077,7 +6084,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -6096,8 +6103,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -6118,7 +6125,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6142,7 +6149,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -6171,7 +6178,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -6211,7 +6218,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="78" thickBot="1">
+    <row r="14" spans="1:10" ht="86" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -6240,7 +6247,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -6264,7 +6271,7 @@
         <v>0.99999999999999978</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -6293,7 +6300,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -6337,6 +6344,79 @@
       </c>
       <c r="J19" t="s">
         <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1"/>
+    <row r="21" spans="1:10" ht="30" thickBot="1">
+      <c r="A21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1">
+      <c r="A22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.13036210000000001</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.86963789999999996</v>
+      </c>
+      <c r="D22" s="6">
+        <f>SUM(B22:C22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="8">
+        <f t="shared" ref="B23:C23" si="2">ROUND(2000*B22,0)</f>
+        <v>261</v>
+      </c>
+      <c r="C23" s="8">
+        <f t="shared" si="2"/>
+        <v>1739</v>
+      </c>
+      <c r="D23" s="8">
+        <f>SUM(B23:C23)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="10">
+        <f>ROUND(2200*B22,0)</f>
+        <v>287</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" ref="C24" si="3">ROUND(2200*C22,0)</f>
+        <v>1913</v>
+      </c>
+      <c r="D24" s="10">
+        <f>SUM(B24:C24)</f>
+        <v>2200</v>
+      </c>
+      <c r="I24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J24" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="J25" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -6345,22 +6425,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -6375,7 +6455,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6393,7 +6473,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -6413,7 +6493,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="27" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -6444,7 +6524,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -6453,7 +6533,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -6474,7 +6554,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6498,7 +6578,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -6527,7 +6607,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" thickBot="1">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -6556,8 +6636,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
@@ -6575,7 +6655,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -6595,7 +6675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -6620,7 +6700,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="27" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -6650,7 +6730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="27" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
@@ -6670,7 +6750,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
@@ -6694,7 +6774,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -6723,7 +6803,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
@@ -6761,7 +6841,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="13" t="s">
         <v>76</v>
       </c>
@@ -6772,7 +6852,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
@@ -6787,7 +6867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>11</v>
       </c>
@@ -6804,7 +6884,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="27" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
@@ -6832,16 +6912,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -6855,7 +6935,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6875,7 +6955,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -6894,7 +6974,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -6913,8 +6993,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -6935,7 +7015,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6959,7 +7039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -6988,7 +7068,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -7028,7 +7108,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -7057,7 +7137,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -7087,7 +7167,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -7122,7 +7202,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -7189,22 +7269,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
@@ -7230,7 +7310,7 @@
       <c r="K1" s="10"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7263,7 +7343,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -7297,7 +7377,7 @@
       <c r="K3" s="10"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -7347,7 +7427,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.6" customHeight="1">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -7361,14 +7441,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -7388,7 +7468,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -7411,7 +7491,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -7436,7 +7516,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -7477,7 +7557,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -7491,7 +7571,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
@@ -7517,7 +7597,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -7546,7 +7626,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -7580,7 +7660,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -7630,7 +7710,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -7644,7 +7724,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="27" thickBot="1">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
@@ -7668,7 +7748,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
@@ -7694,7 +7774,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -7725,7 +7805,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -7756,7 +7836,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
@@ -7766,7 +7846,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="5"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -7791,7 +7871,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>10</v>
       </c>
@@ -7810,7 +7890,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="5" t="s">
         <v>11</v>
       </c>
@@ -7832,7 +7912,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>88</v>
       </c>
@@ -7851,7 +7931,7 @@
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>87</v>
       </c>
@@ -7873,7 +7953,7 @@
       </c>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:12" ht="27" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>89</v>
       </c>
@@ -7906,12 +7986,12 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="27" thickBot="1">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="5" t="s">
         <v>1</v>
       </c>
@@ -7941,7 +8021,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="5" t="s">
         <v>10</v>
       </c>
@@ -7974,7 +8054,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="5" t="s">
         <v>11</v>
       </c>
@@ -8015,7 +8095,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
@@ -8082,12 +8162,12 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>64</v>
       </c>
@@ -8108,7 +8188,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="5" t="s">
         <v>10</v>
       </c>
@@ -8132,7 +8212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="5" t="s">
         <v>11</v>
       </c>
@@ -8161,7 +8241,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="5" t="s">
         <v>12</v>
       </c>
@@ -8217,16 +8297,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -8240,7 +8320,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -8261,7 +8341,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -8282,7 +8362,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -8301,8 +8381,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -8323,7 +8403,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -8347,7 +8427,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -8376,7 +8456,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -8416,7 +8496,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:11" ht="27" thickBot="1">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -8442,7 +8522,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -8472,7 +8552,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -8507,7 +8587,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="27" thickBot="1">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -8557,7 +8637,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75">
+    <row r="19" spans="1:11" ht="16">
       <c r="J19" t="s">
         <v>234</v>
       </c>
@@ -8565,7 +8645,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>76</v>
       </c>
@@ -8579,7 +8659,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27" thickBot="1">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -8597,7 +8677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -8624,7 +8704,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="27" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -8658,23 +8738,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -8688,7 +8768,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="27" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -8709,7 +8789,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -8730,7 +8810,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -8749,8 +8829,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -8771,7 +8851,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="27" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -8795,7 +8875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -8824,7 +8904,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -8864,7 +8944,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="27" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -8884,7 +8964,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -8908,7 +8988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -8937,7 +9017,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="27" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -8981,7 +9061,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="A19" s="13" t="s">
         <v>76</v>
       </c>
@@ -8992,7 +9072,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="27" thickBot="1">
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -9007,7 +9087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -9024,7 +9104,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="27" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -9046,8 +9126,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="25" spans="1:10" ht="39.75" thickBot="1">
+    <row r="24" spans="1:10" ht="16" thickBot="1"/>
+    <row r="25" spans="1:10" ht="44" thickBot="1">
       <c r="A25" s="9" t="s">
         <v>85</v>
       </c>
@@ -9062,7 +9142,7 @@
       </c>
       <c r="E25" s="12"/>
     </row>
-    <row r="26" spans="1:10" ht="27" thickBot="1">
+    <row r="26" spans="1:10" ht="30" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
@@ -9080,7 +9160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" thickBot="1">
+    <row r="27" spans="1:10" ht="16" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>11</v>
       </c>
@@ -9101,7 +9181,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="39.75" thickBot="1">
+    <row r="28" spans="1:10" ht="44" thickBot="1">
       <c r="A28" s="5" t="s">
         <v>89</v>
       </c>
@@ -9143,16 +9223,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -9166,7 +9246,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="27" thickBot="1">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -9187,7 +9267,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -9208,7 +9288,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="27" thickBot="1">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -9227,8 +9307,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -9249,7 +9329,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:13" ht="27" thickBot="1">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -9273,7 +9353,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -9302,7 +9382,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="27" thickBot="1">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -9342,7 +9422,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="27" thickBot="1">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -9371,7 +9451,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="27" thickBot="1">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -9402,7 +9482,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -9438,7 +9518,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="27" thickBot="1">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -9497,8 +9577,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:13" ht="27" thickBot="1">
+    <row r="19" spans="1:13" ht="16" thickBot="1"/>
+    <row r="20" spans="1:13" ht="30" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>85</v>
       </c>
@@ -9510,7 +9590,7 @@
       </c>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:13" ht="27" thickBot="1">
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -9525,7 +9605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" thickBot="1">
+    <row r="22" spans="1:13" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -9542,7 +9622,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="39.75" thickBot="1">
+    <row r="23" spans="1:13" ht="44" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>89</v>
       </c>
@@ -9567,12 +9647,12 @@
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75" thickBot="1">
+    <row r="28" spans="1:13" ht="16" thickBot="1">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="27" thickBot="1">
+    <row r="29" spans="1:13" ht="30" thickBot="1">
       <c r="A29" s="9" t="s">
         <v>85</v>
       </c>
@@ -9585,7 +9665,7 @@
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
     </row>
-    <row r="30" spans="1:13" ht="27" thickBot="1">
+    <row r="30" spans="1:13" ht="30" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>10</v>
       </c>
@@ -9601,7 +9681,7 @@
       </c>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75" thickBot="1">
+    <row r="31" spans="1:13" ht="16" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>11</v>
       </c>
@@ -9619,7 +9699,7 @@
       </c>
       <c r="E31" s="20"/>
     </row>
-    <row r="32" spans="1:13" ht="39.75" thickBot="1">
+    <row r="32" spans="1:13" ht="44" thickBot="1">
       <c r="A32" s="5" t="s">
         <v>89</v>
       </c>
@@ -9652,19 +9732,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -9678,7 +9758,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -9699,7 +9779,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -9720,7 +9800,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -9739,8 +9819,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -9761,7 +9841,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -9785,7 +9865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -9814,7 +9894,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -9863,7 +9943,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="29"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -9886,7 +9966,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -9917,7 +9997,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -9953,7 +10033,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -10020,7 +10100,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1">
       <c r="A21" s="13" t="s">
         <v>76</v>
       </c>
@@ -10031,7 +10111,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="27" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -10046,7 +10126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -10063,7 +10143,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="27" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -10092,16 +10172,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -10115,7 +10195,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -10136,7 +10216,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -10157,7 +10237,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -10176,8 +10256,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -10198,7 +10278,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -10222,7 +10302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -10251,7 +10331,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -10296,7 +10376,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -10322,7 +10402,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -10352,7 +10432,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -10387,7 +10467,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -10434,8 +10514,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="21" spans="1:11" ht="27" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1"/>
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
@@ -10450,7 +10530,7 @@
       </c>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="27" thickBot="1">
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -10468,7 +10548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -10492,7 +10572,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="39.75" thickBot="1">
+    <row r="24" spans="1:11" ht="44" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -10531,16 +10611,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -10554,7 +10634,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="27" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -10575,7 +10655,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -10596,7 +10676,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -10615,8 +10695,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -10637,7 +10717,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="27" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -10661,7 +10741,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -10690,7 +10770,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -10730,7 +10810,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -10753,7 +10833,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -10783,7 +10863,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -10818,7 +10898,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="27" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -10865,8 +10945,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:10" ht="27" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>85</v>
       </c>
@@ -10879,7 +10959,7 @@
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:10" ht="27" thickBot="1">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -10895,7 +10975,7 @@
       </c>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -10913,7 +10993,7 @@
       </c>
       <c r="E22" s="20"/>
     </row>
-    <row r="23" spans="1:10" ht="39.75" thickBot="1">
+    <row r="23" spans="1:10" ht="44" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Add UA zip + Fix typo for TR in preparation.R
</commit_message>
<xml_diff>
--- a/questionnaires/quotas.xlsx
+++ b/questionnaires/quotas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC947039-CED4-AA4F-9A50-A56CBFF236D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F824CBD0-8889-9F4C-8C58-DC8ACF611642}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="3380" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="6" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="8" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotas_US" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="323">
   <si>
     <t>IDF</t>
   </si>
@@ -1025,6 +1025,12 @@
   </si>
   <si>
     <t>file "2020년 도시지역 인구현황(시군구별).xls"</t>
+  </si>
+  <si>
+    <t>http://www.ukrstat.gov.ua/druk/publicat/kat_u/2020/zb/05/zb_chuselnist%202019.pdf</t>
+  </si>
+  <si>
+    <t>(page 5)</t>
   </si>
 </sst>
 </file>
@@ -4843,7 +4849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -6153,7 +6159,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -7040,10 +7046,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -7388,6 +7394,79 @@
       </c>
       <c r="K19" t="s">
         <v>293</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" thickBot="1"/>
+    <row r="21" spans="1:11" ht="30" thickBot="1">
+      <c r="A21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" ht="16" thickBot="1">
+      <c r="A22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.30459999999999998</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.69540000000000002</v>
+      </c>
+      <c r="D22" s="6">
+        <f>SUM(B22:C22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="8">
+        <f t="shared" ref="B23:C23" si="2">ROUND(2000*B22,0)</f>
+        <v>609</v>
+      </c>
+      <c r="C23" s="8">
+        <f t="shared" si="2"/>
+        <v>1391</v>
+      </c>
+      <c r="D23" s="8">
+        <f>SUM(B23:C23)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="10">
+        <f>ROUND(2200*B22,0)</f>
+        <v>670</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" ref="C24" si="3">ROUND(2200*C22,0)</f>
+        <v>1530</v>
+      </c>
+      <c r="D24" s="10">
+        <f>SUM(B24:C24)</f>
+        <v>2200</v>
+      </c>
+      <c r="I24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J24" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="J25" t="s">
+        <v>322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add urban categories BR
</commit_message>
<xml_diff>
--- a/questionnaires/quotas.xlsx
+++ b/questionnaires/quotas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F824CBD0-8889-9F4C-8C58-DC8ACF611642}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214BDF1E-40E6-9B41-8749-D38F38D1F325}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="8" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotas_US" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="quota_TR" sheetId="21" r:id="rId19"/>
     <sheet name="quota_UA" sheetId="22" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="326">
   <si>
     <t>IDF</t>
   </si>
@@ -1031,6 +1031,15 @@
   </si>
   <si>
     <t>(page 5)</t>
+  </si>
+  <si>
+    <t>Municipality &lt;50k</t>
+  </si>
+  <si>
+    <t>Municipality &gt;50k</t>
+  </si>
+  <si>
+    <t>https://www.caurj.gov.br/populacao-brasileira-chega-a-2118-milhoes-de-habitantes-em-2020/</t>
   </si>
 </sst>
 </file>
@@ -4049,10 +4058,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -4366,6 +4375,74 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1"/>
+    <row r="21" spans="1:10" ht="30" thickBot="1">
+      <c r="A21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>323</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1">
+      <c r="A22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.3099137235942635</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.6900862764057365</v>
+      </c>
+      <c r="D22" s="6">
+        <f>SUM(B22:C22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="8">
+        <f t="shared" ref="B23:C23" si="2">ROUND(2000*B22,0)</f>
+        <v>620</v>
+      </c>
+      <c r="C23" s="8">
+        <f t="shared" si="2"/>
+        <v>1380</v>
+      </c>
+      <c r="D23" s="8">
+        <f>SUM(B23:C23)</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="10">
+        <f>ROUND(2200*B22,0)</f>
+        <v>682</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" ref="C24" si="3">ROUND(2200*C22,0)</f>
+        <v>1518</v>
+      </c>
+      <c r="D24" s="10">
+        <f>SUM(B24:C24)</f>
+        <v>2200</v>
+      </c>
+      <c r="I24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J24" t="s">
+        <v>325</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7048,8 +7125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Merge Regions UA, TR, SK
</commit_message>
<xml_diff>
--- a/questionnaires/quotas.xlsx
+++ b/questionnaires/quotas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afabre\Documents\www\oecd_climate\questionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A26EC504-B7F2-514B-913D-64876403B1A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14475" tabRatio="923" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="15" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotas_US" sheetId="2" r:id="rId1"/>
@@ -33,7 +34,7 @@
     <sheet name="quota_TR" sheetId="21" r:id="rId19"/>
     <sheet name="quota_UA" sheetId="22" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="336">
   <si>
     <t>IDF</t>
   </si>
@@ -903,12 +904,6 @@
     <t>Mediterranean</t>
   </si>
   <si>
-    <t>Aegean</t>
-  </si>
-  <si>
-    <t>Black Sea</t>
-  </si>
-  <si>
     <t>Anatolia:</t>
   </si>
   <si>
@@ -1063,12 +1058,24 @@
   </si>
   <si>
     <t>* The quota count was badly coded on qualtrics, implying the 4 extra Central counts.</t>
+  </si>
+  <si>
+    <t>North West:</t>
+  </si>
+  <si>
+    <t>Aegean + Black Sea</t>
+  </si>
+  <si>
+    <t>Central-West (0,109) + South-West (0,111)</t>
+  </si>
+  <si>
+    <t>Center-East (0,082) + Center-West (0,229)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -1297,7 +1304,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1574,14 +1581,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -2070,24 +2077,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D22" r:id="rId2" display="https://www.ers.usda.gov/data-products/rural-urban-commuting-area-codes/" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -2101,7 +2108,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -2121,7 +2128,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2140,7 +2147,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -2159,8 +2166,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -2181,7 +2188,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2205,7 +2212,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -2274,7 +2281,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -2303,7 +2310,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -2365,7 +2372,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -2420,8 +2427,8 @@
         <v>267</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="23" spans="1:10" ht="27" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1"/>
+    <row r="23" spans="1:10" ht="30" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>85</v>
       </c>
@@ -2434,7 +2441,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1">
+    <row r="24" spans="1:10" ht="16" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -2453,10 +2460,10 @@
         <v>211</v>
       </c>
       <c r="G24" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="16" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
@@ -2477,10 +2484,10 @@
         <v>171</v>
       </c>
       <c r="G25" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="39.75" thickBot="1">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="44" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>89</v>
       </c>
@@ -2498,12 +2505,12 @@
       </c>
       <c r="E26" s="20"/>
       <c r="G26" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="G27" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -2512,21 +2519,21 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -2541,7 +2548,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -2563,7 +2570,7 @@
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -2585,7 +2592,7 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -2626,7 +2633,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="25"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9"/>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -2636,7 +2643,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="25"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
@@ -2658,7 +2665,7 @@
       <c r="G8" s="7"/>
       <c r="H8" s="25"/>
     </row>
-    <row r="9" spans="1:11" ht="27" thickBot="1">
+    <row r="9" spans="1:11" ht="30" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -2683,7 +2690,7 @@
       </c>
       <c r="H9" s="25"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+    <row r="10" spans="1:11" ht="16" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -2713,7 +2720,7 @@
       </c>
       <c r="H10" s="25"/>
     </row>
-    <row r="11" spans="1:11" ht="27" thickBot="1">
+    <row r="11" spans="1:11" ht="30" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -2758,7 +2765,7 @@
     <row r="13" spans="1:11">
       <c r="H13" s="25"/>
     </row>
-    <row r="14" spans="1:11" ht="65.25" thickBot="1">
+    <row r="14" spans="1:11" ht="72" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -2772,7 +2779,7 @@
         <v>119</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>120</v>
@@ -2780,10 +2787,10 @@
       <c r="G14" s="29"/>
       <c r="H14" s="25"/>
       <c r="K14" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -2807,7 +2814,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -2839,7 +2846,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="27" thickBot="1">
+    <row r="17" spans="1:12" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -2908,15 +2915,15 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="27" thickBot="1">
+    <row r="21" spans="1:12" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>218</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -2924,7 +2931,7 @@
       <c r="G21" s="29"/>
       <c r="H21" s="25"/>
     </row>
-    <row r="22" spans="1:12" ht="27" thickBot="1">
+    <row r="22" spans="1:12" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -2943,7 +2950,7 @@
       <c r="E22" s="21"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -2963,7 +2970,7 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:12" ht="27" thickBot="1">
+    <row r="24" spans="1:12" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -3009,7 +3016,7 @@
       <c r="E27" s="11"/>
       <c r="H27" s="25"/>
     </row>
-    <row r="28" spans="1:12" ht="27" thickBot="1">
+    <row r="28" spans="1:12" ht="30" thickBot="1">
       <c r="A28" s="9" t="s">
         <v>218</v>
       </c>
@@ -3033,7 +3040,7 @@
       </c>
       <c r="H28" s="25"/>
     </row>
-    <row r="29" spans="1:12" ht="27" thickBot="1">
+    <row r="29" spans="1:12" ht="30" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>10</v>
       </c>
@@ -3060,7 +3067,7 @@
         <v>0.99989215000000009</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>11</v>
       </c>
@@ -3093,7 +3100,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="27" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
@@ -3182,16 +3189,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -3205,7 +3212,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -3226,7 +3233,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -3247,7 +3254,7 @@
         <v>0.99792841994678028</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27.75" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -3266,8 +3273,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="34"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -3288,7 +3295,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -3312,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -3341,7 +3348,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -3381,7 +3388,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="27" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -3410,7 +3417,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -3440,7 +3447,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -3475,7 +3482,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -3530,8 +3537,8 @@
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="23" spans="1:11" ht="27" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1"/>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="9" t="s">
         <v>85</v>
       </c>
@@ -3544,7 +3551,7 @@
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
     </row>
-    <row r="24" spans="1:11" ht="27" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>10</v>
       </c>
@@ -3566,7 +3573,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1">
+    <row r="25" spans="1:11" ht="16" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>11</v>
       </c>
@@ -3590,7 +3597,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="39.75" thickBot="1">
+    <row r="26" spans="1:11" ht="44" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>89</v>
       </c>
@@ -3615,16 +3622,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -3638,7 +3645,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+    <row r="2" spans="1:11" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -3659,7 +3666,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -3680,7 +3687,7 @@
         <v>0.97760081385085629</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -3699,8 +3706,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -3721,7 +3728,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+    <row r="8" spans="1:11" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -3745,7 +3752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -3774,7 +3781,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -3814,7 +3821,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -3837,7 +3844,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -3867,7 +3874,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -3902,7 +3909,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -3952,8 +3959,8 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="22" spans="1:11" ht="27" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>85</v>
       </c>
@@ -3966,7 +3973,7 @@
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
@@ -3988,7 +3995,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
@@ -4015,7 +4022,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="39.75" thickBot="1">
+    <row r="25" spans="1:11" ht="44" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
@@ -4039,16 +4046,16 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -4062,7 +4069,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4083,7 +4090,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -4104,7 +4111,7 @@
         <v>1.0341140064832992</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -4123,8 +4130,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -4145,7 +4152,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4169,7 +4176,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -4198,7 +4205,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -4238,7 +4245,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="27" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -4252,7 +4259,7 @@
         <v>256</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>48</v>
@@ -4261,7 +4268,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -4291,7 +4298,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -4326,7 +4333,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="27" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -4364,7 +4371,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1">
+    <row r="19" spans="1:9" ht="16" thickBot="1">
       <c r="A19" s="13" t="s">
         <v>76</v>
       </c>
@@ -4375,7 +4382,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1">
+    <row r="20" spans="1:9" ht="16" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
@@ -4396,7 +4403,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1">
+    <row r="21" spans="1:9" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -4413,7 +4420,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="27" thickBot="1">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>12</v>
       </c>
@@ -4541,16 +4548,16 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -4564,7 +4571,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4585,7 +4592,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -4606,7 +4613,7 @@
         <v>0.95217958067188335</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="27" thickBot="1">
+    <row r="4" spans="1:7" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -4625,8 +4632,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1"/>
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -4647,7 +4654,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -4671,7 +4678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -4700,7 +4707,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" thickBot="1">
+    <row r="10" spans="1:7" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -4740,7 +4747,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -4763,7 +4770,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -4787,7 +4794,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1">
+    <row r="16" spans="1:7" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -4816,7 +4823,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -4848,7 +4855,7 @@
         <v>234</v>
       </c>
       <c r="J17" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -4860,20 +4867,20 @@
       <c r="D18" s="2"/>
       <c r="E18" s="11"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="21" spans="1:10" ht="27" thickBot="1">
+    <row r="20" spans="1:10" ht="16" thickBot="1"/>
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -4888,7 +4895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -4905,7 +4912,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="27" thickBot="1">
+    <row r="24" spans="1:10" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -4925,7 +4932,7 @@
         <v>234</v>
       </c>
       <c r="J24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -4934,16 +4941,16 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="D23" sqref="A20:D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -4957,7 +4964,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -4977,7 +4984,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -4996,7 +5003,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -5015,8 +5022,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -5037,7 +5044,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5061,7 +5068,7 @@
         <v>0.99999999999999944</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -5090,7 +5097,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -5130,7 +5137,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -5159,7 +5166,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -5189,7 +5196,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -5221,7 +5228,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -5268,7 +5275,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1">
       <c r="I19" t="s">
         <v>234</v>
       </c>
@@ -5276,7 +5283,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="27" thickBot="1">
+    <row r="20" spans="1:10" ht="30" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>85</v>
       </c>
@@ -5288,7 +5295,7 @@
       </c>
       <c r="D20" s="12"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -5303,7 +5310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -5320,7 +5327,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="27" thickBot="1">
+    <row r="23" spans="1:10" ht="30" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -5340,7 +5347,7 @@
         <v>234</v>
       </c>
       <c r="J23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -5349,16 +5356,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="B22" sqref="B22:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -5372,7 +5379,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -5393,7 +5400,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5414,7 +5421,7 @@
         <v>0.92970833595125124</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -5433,8 +5440,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -5455,7 +5462,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5479,7 +5486,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -5508,7 +5515,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -5548,7 +5555,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -5577,7 +5584,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -5607,7 +5614,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -5642,7 +5649,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -5700,7 +5707,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="13" t="s">
         <v>76</v>
       </c>
@@ -5708,13 +5715,13 @@
         <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -5732,7 +5739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -5753,13 +5760,13 @@
         <v>2000</v>
       </c>
       <c r="F23" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G23" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="27" thickBot="1">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -5783,7 +5790,7 @@
         <v>208</v>
       </c>
       <c r="G24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -5794,15 +5801,15 @@
         <v>214</v>
       </c>
       <c r="H25" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="G26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="H26" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5810,7 +5817,7 @@
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -5822,16 +5829,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -5845,7 +5852,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -5866,7 +5873,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -5887,7 +5894,7 @@
         <v>1.01</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -5906,8 +5913,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -5928,7 +5935,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -5952,7 +5959,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -5981,7 +5988,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -6021,7 +6028,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -6032,13 +6039,13 @@
         <v>133</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>256</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="G14" s="29" t="s">
         <v>139</v>
@@ -6047,7 +6054,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -6058,17 +6065,18 @@
         <v>0.343251015277311</v>
       </c>
       <c r="D15" s="31">
-        <v>0.10921309468591101</v>
+        <v>0.22025659607004799</v>
       </c>
       <c r="E15" s="31">
-        <v>0.111043501384137</v>
-      </c>
-      <c r="F15" s="31">
         <v>0.25032612031513901</v>
+      </c>
+      <c r="F15" s="17">
+        <f>SUM(A15:E15)</f>
+        <v>1</v>
       </c>
       <c r="G15" s="17">
         <f>SUM(B15:F15)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" t="s">
         <v>133</v>
@@ -6077,7 +6085,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -6091,19 +6099,19 @@
       </c>
       <c r="D16" s="10">
         <f>ROUND(2000*D15,0)</f>
-        <v>218</v>
+        <v>441</v>
       </c>
       <c r="E16" s="10">
         <f>ROUND(2000*E15,0)</f>
-        <v>222</v>
-      </c>
-      <c r="F16" s="10">
-        <f>ROUND(2000*F15,0)</f>
         <v>501</v>
+      </c>
+      <c r="F16" s="3">
+        <f>SUM(A16:E16)</f>
+        <v>2001</v>
       </c>
       <c r="G16" s="3">
         <f>SUM(B16:F16)</f>
-        <v>2000</v>
+        <v>4002</v>
       </c>
       <c r="I16" t="s">
         <v>244</v>
@@ -6112,7 +6120,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -6126,19 +6134,19 @@
       </c>
       <c r="D17" s="2">
         <f>ROUND(2200*D15,0)</f>
-        <v>240</v>
+        <v>485</v>
       </c>
       <c r="E17" s="2">
         <f>ROUND(2200*E15,0)</f>
-        <v>244</v>
-      </c>
-      <c r="F17" s="2">
-        <f>ROUND(2200*F15,0)</f>
         <v>551</v>
+      </c>
+      <c r="F17" s="3">
+        <f>SUM(A17:E17)</f>
+        <v>2201</v>
       </c>
       <c r="G17" s="3">
         <f>SUM(B17:F17)</f>
-        <v>2200</v>
+        <v>4402</v>
       </c>
       <c r="I17" t="s">
         <v>112</v>
@@ -6170,21 +6178,29 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+    <row r="20" spans="1:10">
+      <c r="I20" t="s">
+        <v>176</v>
+      </c>
+      <c r="J20" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="16" thickBot="1">
       <c r="A21" s="13" t="s">
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C21" t="s">
         <v>188</v>
       </c>
       <c r="D21" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -6202,10 +6218,10 @@
         <v>1.0000000099999999</v>
       </c>
       <c r="H22" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -6229,10 +6245,10 @@
         <v>140</v>
       </c>
       <c r="H23" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="27" thickBot="1">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -6257,7 +6273,7 @@
       </c>
       <c r="G24" s="15"/>
       <c r="H24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -6268,12 +6284,12 @@
         <v>234</v>
       </c>
       <c r="I25" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="I26" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -6282,16 +6298,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -6305,7 +6321,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6325,7 +6341,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -6344,7 +6360,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -6363,8 +6379,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -6385,7 +6401,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6409,7 +6425,7 @@
         <v>0.99999999999999933</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -6438,7 +6454,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -6478,7 +6494,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="78" thickBot="1">
+    <row r="14" spans="1:10" ht="86" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -6492,22 +6508,19 @@
         <v>279</v>
       </c>
       <c r="E14" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="I14" s="29" t="s">
         <v>280</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="J14" s="29" t="s">
         <v>281</v>
       </c>
-      <c r="G14" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="I14" s="29" t="s">
-        <v>282</v>
-      </c>
-      <c r="J14" s="29" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -6521,17 +6534,20 @@
         <v>0.13099525360860201</v>
       </c>
       <c r="E15" s="16">
-        <v>0.128080832149781</v>
-      </c>
-      <c r="F15" s="16">
-        <v>9.5264671201471807E-2</v>
-      </c>
-      <c r="G15" s="17">
-        <f>SUM(B15:F15)</f>
+        <v>0.22334550335125281</v>
+      </c>
+      <c r="F15" s="17">
+        <f ca="1">SUM(B15:F15)</f>
         <v>0.99999999999999978</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+      <c r="I15" t="s">
+        <v>332</v>
+      </c>
+      <c r="J15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -6549,18 +6565,14 @@
       </c>
       <c r="E16" s="10">
         <f>ROUND(2000*E15,0)</f>
-        <v>256</v>
-      </c>
-      <c r="F16" s="10">
-        <f>ROUND(2000*F15,0)</f>
-        <v>191</v>
-      </c>
-      <c r="G16" s="3">
-        <f>SUM(B16:F16)</f>
+        <v>447</v>
+      </c>
+      <c r="F16" s="3">
+        <f ca="1">SUM(B16:F16)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="27" thickBot="1">
+    <row r="17" spans="1:10" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -6578,15 +6590,11 @@
       </c>
       <c r="E17" s="2">
         <f>ROUND(2200*E15,0)</f>
-        <v>282</v>
-      </c>
-      <c r="F17" s="2">
-        <f>ROUND(2200*F15,0)</f>
-        <v>210</v>
-      </c>
-      <c r="G17" s="3">
-        <f>SUM(B17:F17)</f>
-        <v>2200</v>
+        <v>491</v>
+      </c>
+      <c r="F17" s="3">
+        <f ca="1">SUM(B17:F17)</f>
+        <v>2199</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -6603,11 +6611,11 @@
         <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="21" spans="1:10" ht="27" thickBot="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="16" thickBot="1"/>
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
@@ -6619,7 +6627,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -6634,7 +6642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -6651,7 +6659,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="27" thickBot="1">
+    <row r="24" spans="1:10" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -6671,12 +6679,12 @@
         <v>234</v>
       </c>
       <c r="J24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="J25" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -6685,22 +6693,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -6715,7 +6723,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1">
+    <row r="2" spans="1:7" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -6733,7 +6741,7 @@
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+    <row r="3" spans="1:7" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -6753,7 +6761,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" ht="27" thickBot="1">
+    <row r="4" spans="1:7" ht="16" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -6784,7 +6792,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1">
+    <row r="6" spans="1:7" ht="16" thickBot="1">
       <c r="A6" s="2"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -6793,7 +6801,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1">
+    <row r="7" spans="1:7" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -6814,7 +6822,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1">
+    <row r="8" spans="1:7" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -6838,7 +6846,7 @@
         <v>1.0001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1">
+    <row r="9" spans="1:7" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -6867,7 +6875,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27" thickBot="1">
+    <row r="10" spans="1:7" ht="16" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -6896,8 +6904,8 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1"/>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1">
+    <row r="11" spans="1:7" ht="16" thickBot="1"/>
+    <row r="12" spans="1:7" ht="16" thickBot="1">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
@@ -6915,7 +6923,7 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1">
+    <row r="13" spans="1:7" ht="16" thickBot="1">
       <c r="A13" s="5" t="s">
         <v>28</v>
       </c>
@@ -6935,7 +6943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1">
+    <row r="14" spans="1:7" ht="16" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -6960,7 +6968,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="27" thickBot="1">
+    <row r="15" spans="1:7" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -6990,7 +6998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="27" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="9" t="s">
         <v>13</v>
       </c>
@@ -7010,7 +7018,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="5" t="s">
         <v>10</v>
       </c>
@@ -7034,7 +7042,7 @@
         <v>0.99990000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -7063,7 +7071,7 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="27" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>12</v>
       </c>
@@ -7101,7 +7109,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="11"/>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="13" t="s">
         <v>76</v>
       </c>
@@ -7112,7 +7120,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>10</v>
       </c>
@@ -7127,7 +7135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:7" ht="16" thickBot="1">
       <c r="A26" s="5" t="s">
         <v>11</v>
       </c>
@@ -7144,7 +7152,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="27" thickBot="1">
+    <row r="27" spans="1:7" ht="16" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>12</v>
       </c>
@@ -7172,16 +7180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -7195,7 +7203,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1">
+    <row r="2" spans="1:10" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7215,7 +7223,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -7234,7 +7242,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -7253,8 +7261,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -7275,7 +7283,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1">
+    <row r="8" spans="1:10" ht="16" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -7299,7 +7307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -7328,7 +7336,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -7368,133 +7376,119 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>285</v>
+        <v>175</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>286</v>
+        <v>256</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>256</v>
-      </c>
-      <c r="E14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="F14" s="29" t="s">
         <v>139</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="J14" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="31">
-        <v>8.2140396161971399E-2</v>
+        <v>0.31130874366166739</v>
       </c>
       <c r="C15" s="31">
-        <v>0.229168347499696</v>
+        <v>0.21309541835208201</v>
       </c>
       <c r="D15" s="31">
-        <v>0.21309541835208201</v>
+        <v>0.22456565856781299</v>
       </c>
       <c r="E15" s="31">
-        <v>0.22456565856781299</v>
-      </c>
-      <c r="F15" s="31">
         <v>0.25103017941843703</v>
       </c>
-      <c r="G15" s="17">
-        <f>SUM(B15:F15)</f>
+      <c r="F15" s="17">
+        <f>SUM(B15:E15)</f>
         <v>0.99999999999999933</v>
       </c>
       <c r="I15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J15" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="10">
         <f>ROUND(2000*B15,0)</f>
-        <v>164</v>
+        <v>623</v>
       </c>
       <c r="C16" s="10">
         <f>ROUND(2000*C15,0)</f>
-        <v>458</v>
+        <v>426</v>
       </c>
       <c r="D16" s="10">
         <f>ROUND(2000*D15,0)</f>
-        <v>426</v>
+        <v>449</v>
       </c>
       <c r="E16" s="10">
         <f>ROUND(2000*E15,0)</f>
-        <v>449</v>
-      </c>
-      <c r="F16" s="10">
-        <f>ROUND(2000*F15,0)</f>
         <v>502</v>
       </c>
-      <c r="G16" s="3">
-        <f>SUM(B16:F16)</f>
-        <v>1999</v>
+      <c r="F16" s="3">
+        <f>SUM(B16:E16)</f>
+        <v>2000</v>
       </c>
       <c r="I16" t="s">
         <v>256</v>
       </c>
       <c r="J16" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="2">
         <f>ROUND(2200*B15,0)</f>
-        <v>181</v>
+        <v>685</v>
       </c>
       <c r="C17" s="2">
         <f>ROUND(2200*C15,0)</f>
-        <v>504</v>
+        <v>469</v>
       </c>
       <c r="D17" s="2">
         <f>ROUND(2200*D15,0)</f>
-        <v>469</v>
+        <v>494</v>
       </c>
       <c r="E17" s="2">
         <f>ROUND(2200*E15,0)</f>
-        <v>494</v>
-      </c>
-      <c r="F17" s="2">
-        <f>ROUND(2200*F15,0)</f>
         <v>552</v>
       </c>
-      <c r="G17" s="3">
-        <f>SUM(B17:F17)</f>
+      <c r="F17" s="3">
+        <f>SUM(B17:E17)</f>
         <v>2200</v>
       </c>
       <c r="I17" t="s">
         <v>47</v>
       </c>
       <c r="J17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -7509,7 +7503,7 @@
         <v>48</v>
       </c>
       <c r="J18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -7517,14 +7511,21 @@
         <v>234</v>
       </c>
       <c r="J19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="K19" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="21" spans="1:11" ht="27" thickBot="1">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" thickBot="1">
+      <c r="I20" t="s">
+        <v>131</v>
+      </c>
+      <c r="J20" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
@@ -7536,7 +7537,7 @@
       </c>
       <c r="D21" s="12"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -7551,7 +7552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
+    <row r="23" spans="1:11" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -7568,7 +7569,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="27" thickBot="1">
+    <row r="24" spans="1:11" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>12</v>
       </c>
@@ -7588,12 +7589,12 @@
         <v>234</v>
       </c>
       <c r="J24" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="J25" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -7602,22 +7603,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27" thickBot="1">
+    <row r="1" spans="1:12" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>59</v>
       </c>
@@ -7643,7 +7644,7 @@
       <c r="K1" s="10"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -7676,7 +7677,7 @@
       <c r="K2" s="10"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1">
+    <row r="3" spans="1:12" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -7710,7 +7711,7 @@
       <c r="K3" s="10"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1">
+    <row r="4" spans="1:12" ht="16" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -7760,7 +7761,7 @@
       <c r="K5" s="10"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="0.6" customHeight="1">
+    <row r="6" spans="1:12" ht="0.5" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -7774,14 +7775,14 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1">
+    <row r="7" spans="1:12" ht="16" thickBot="1">
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1">
+    <row r="8" spans="1:12" ht="16" thickBot="1">
       <c r="A8" s="9" t="s">
         <v>14</v>
       </c>
@@ -7801,7 +7802,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1">
+    <row r="9" spans="1:12" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -7824,7 +7825,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1">
+    <row r="10" spans="1:12" ht="16" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -7849,7 +7850,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1">
+    <row r="11" spans="1:12" ht="16" thickBot="1">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -7890,7 +7891,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1">
+    <row r="13" spans="1:12" ht="16" thickBot="1">
       <c r="A13" s="2"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -7904,7 +7905,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1">
+    <row r="14" spans="1:12" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
@@ -7930,7 +7931,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1">
+    <row r="15" spans="1:12" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -7959,7 +7960,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1">
+    <row r="16" spans="1:12" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -7993,7 +7994,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15.75" thickBot="1">
+    <row r="17" spans="1:12" ht="16" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -8043,7 +8044,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75" thickBot="1">
+    <row r="19" spans="1:12" ht="16" thickBot="1">
       <c r="A19" s="2"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -8057,7 +8058,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="27" thickBot="1">
+    <row r="20" spans="1:12" ht="30" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>23</v>
       </c>
@@ -8081,7 +8082,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" thickBot="1">
+    <row r="21" spans="1:12" ht="16" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>28</v>
       </c>
@@ -8107,7 +8108,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1">
+    <row r="22" spans="1:12" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -8138,7 +8139,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1">
+    <row r="23" spans="1:12" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -8169,7 +8170,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="1:12" ht="15.75" thickBot="1">
+    <row r="24" spans="1:12" ht="16" thickBot="1">
       <c r="A24" s="9" t="s">
         <v>30</v>
       </c>
@@ -8179,7 +8180,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1">
+    <row r="25" spans="1:12" ht="16" thickBot="1">
       <c r="A25" s="5"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -8204,7 +8205,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:12" ht="15.75" thickBot="1">
+    <row r="27" spans="1:12" ht="16" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>10</v>
       </c>
@@ -8223,7 +8224,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:12" ht="15.75" thickBot="1">
+    <row r="28" spans="1:12" ht="16" thickBot="1">
       <c r="A28" s="5" t="s">
         <v>11</v>
       </c>
@@ -8245,7 +8246,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:12" ht="15.75" thickBot="1">
+    <row r="29" spans="1:12" ht="16" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>88</v>
       </c>
@@ -8264,7 +8265,7 @@
       </c>
       <c r="F29" s="10"/>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1">
+    <row r="30" spans="1:12" ht="16" thickBot="1">
       <c r="A30" s="5" t="s">
         <v>87</v>
       </c>
@@ -8286,7 +8287,7 @@
       </c>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:12" ht="27" thickBot="1">
+    <row r="31" spans="1:12" ht="30" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>89</v>
       </c>
@@ -8319,12 +8320,12 @@
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" thickBot="1">
+    <row r="36" spans="1:10" ht="16" thickBot="1">
       <c r="A36" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="27" thickBot="1">
+    <row r="37" spans="1:10" ht="30" thickBot="1">
       <c r="A37" s="5" t="s">
         <v>1</v>
       </c>
@@ -8354,7 +8355,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" thickBot="1">
+    <row r="38" spans="1:10" ht="16" thickBot="1">
       <c r="A38" s="5" t="s">
         <v>10</v>
       </c>
@@ -8387,7 +8388,7 @@
         <v>0.998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" thickBot="1">
+    <row r="39" spans="1:10" ht="16" thickBot="1">
       <c r="A39" s="5" t="s">
         <v>11</v>
       </c>
@@ -8428,7 +8429,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1">
+    <row r="40" spans="1:10" ht="16" thickBot="1">
       <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
@@ -8495,12 +8496,12 @@
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:10" ht="15.75" thickBot="1">
+    <row r="43" spans="1:10" ht="16" thickBot="1">
       <c r="A43" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" thickBot="1">
+    <row r="44" spans="1:10" ht="16" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>64</v>
       </c>
@@ -8521,7 +8522,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:10" ht="15.75" thickBot="1">
+    <row r="45" spans="1:10" ht="16" thickBot="1">
       <c r="A45" s="5" t="s">
         <v>10</v>
       </c>
@@ -8545,7 +8546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" thickBot="1">
+    <row r="46" spans="1:10" ht="16" thickBot="1">
       <c r="A46" s="5" t="s">
         <v>11</v>
       </c>
@@ -8574,7 +8575,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" thickBot="1">
+    <row r="47" spans="1:10" ht="16" thickBot="1">
       <c r="A47" s="5" t="s">
         <v>12</v>
       </c>
@@ -8630,16 +8631,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H26" sqref="A20:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -8653,7 +8654,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -8674,7 +8675,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -8695,7 +8696,7 @@
         <v>0.95277529961698948</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -8714,8 +8715,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -8736,7 +8737,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -8760,7 +8761,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -8789,7 +8790,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -8829,7 +8830,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:11" ht="27" thickBot="1">
+    <row r="13" spans="1:11" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -8855,7 +8856,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -8885,7 +8886,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+    <row r="15" spans="1:11" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -8920,7 +8921,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="27" thickBot="1">
+    <row r="16" spans="1:11" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -8970,7 +8971,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75">
+    <row r="19" spans="1:11" ht="16">
       <c r="J19" t="s">
         <v>234</v>
       </c>
@@ -8978,7 +8979,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1">
+    <row r="20" spans="1:11" ht="16" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>76</v>
       </c>
@@ -8992,7 +8993,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="27" thickBot="1">
+    <row r="21" spans="1:11" ht="30" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -9010,7 +9011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -9037,7 +9038,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="27" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>12</v>
       </c>
@@ -9071,23 +9072,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G23" r:id="rId1"/>
+    <hyperlink ref="G23" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -9101,7 +9102,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="27" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -9122,7 +9123,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -9143,7 +9144,7 @@
         <v>0.90805800128462044</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -9162,8 +9163,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -9184,7 +9185,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="27" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -9208,7 +9209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -9237,7 +9238,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -9277,7 +9278,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="27" thickBot="1">
+    <row r="13" spans="1:10" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -9297,7 +9298,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -9321,10 +9322,10 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -9353,9 +9354,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="27" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B16" s="10">
         <v>528</v>
@@ -9377,9 +9378,9 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="39.75" thickBot="1">
+    <row r="17" spans="1:10" ht="44" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B17" s="2">
         <f>ROUND(1.1*B16,0)</f>
@@ -9421,8 +9422,8 @@
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="20" spans="1:10" ht="39.75" thickBot="1">
+    <row r="19" spans="1:10" ht="16" thickBot="1"/>
+    <row r="20" spans="1:10" ht="44" thickBot="1">
       <c r="A20" s="9" t="s">
         <v>85</v>
       </c>
@@ -9437,7 +9438,7 @@
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:10" ht="27" thickBot="1">
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>10</v>
       </c>
@@ -9455,7 +9456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1">
+    <row r="22" spans="1:10" ht="16" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -9476,9 +9477,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="27" thickBot="1">
+    <row r="23" spans="1:10" ht="30" thickBot="1">
       <c r="A23" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B23" s="10">
         <v>693</v>
@@ -9494,9 +9495,9 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="52.5" thickBot="1">
+    <row r="24" spans="1:10" ht="58" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B24" s="10">
         <f>ROUND(1.1*B23,0)</f>
@@ -9530,7 +9531,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="36" customFormat="1" ht="15.75" thickBot="1">
+    <row r="27" spans="1:10" s="36" customFormat="1" ht="16" thickBot="1">
       <c r="A27" s="35" t="s">
         <v>76</v>
       </c>
@@ -9541,7 +9542,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="36" customFormat="1" ht="27" thickBot="1">
+    <row r="28" spans="1:10" s="36" customFormat="1" ht="30" thickBot="1">
       <c r="A28" s="37" t="s">
         <v>10</v>
       </c>
@@ -9556,7 +9557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="36" customFormat="1" ht="15.75" thickBot="1">
+    <row r="29" spans="1:10" s="36" customFormat="1" ht="16" thickBot="1">
       <c r="A29" s="37" t="s">
         <v>11</v>
       </c>
@@ -9573,9 +9574,9 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="36" customFormat="1" ht="39.75" thickBot="1">
+    <row r="30" spans="1:10" s="36" customFormat="1" ht="44" thickBot="1">
       <c r="A30" s="37" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B30" s="36">
         <f>ROUND(2200*B28,0)</f>
@@ -9603,19 +9604,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -9629,7 +9630,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -9650,7 +9651,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -9671,7 +9672,7 @@
         <v>0.97448244785232785</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -9690,8 +9691,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -9712,7 +9713,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -9736,7 +9737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -9765,7 +9766,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -9814,7 +9815,7 @@
       <c r="F13" s="19"/>
       <c r="G13" s="29"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+    <row r="14" spans="1:11" ht="16" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -9837,7 +9838,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -9868,7 +9869,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -9904,9 +9905,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B17" s="10">
         <v>590</v>
@@ -9935,7 +9936,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="27" thickBot="1">
+    <row r="18" spans="1:11" ht="30" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
@@ -9994,7 +9995,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1">
+    <row r="22" spans="1:11" ht="16" thickBot="1">
       <c r="A22" s="13" t="s">
         <v>76</v>
       </c>
@@ -10005,7 +10006,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="27" thickBot="1">
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
@@ -10020,10 +10021,10 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
@@ -10040,7 +10041,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="27" thickBot="1">
+    <row r="25" spans="1:11" ht="30" thickBot="1">
       <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
@@ -10069,16 +10070,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
+    <row r="1" spans="1:11" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -10092,7 +10093,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="27" thickBot="1">
+    <row r="2" spans="1:11" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -10113,7 +10114,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
+    <row r="3" spans="1:11" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -10134,7 +10135,7 @@
         <v>0.98351979013457747</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" thickBot="1">
+    <row r="4" spans="1:11" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -10153,8 +10154,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:11" ht="16" thickBot="1"/>
+    <row r="7" spans="1:11" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -10175,7 +10176,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="27" thickBot="1">
+    <row r="8" spans="1:11" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -10199,7 +10200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:11" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -10228,7 +10229,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="27" thickBot="1">
+    <row r="10" spans="1:11" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -10273,7 +10274,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="27" thickBot="1">
+    <row r="14" spans="1:11" ht="30" thickBot="1">
       <c r="A14" s="9" t="s">
         <v>13</v>
       </c>
@@ -10299,7 +10300,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="27" thickBot="1">
+    <row r="15" spans="1:11" ht="30" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -10329,7 +10330,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="16" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -10364,9 +10365,9 @@
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="27" thickBot="1">
+    <row r="17" spans="1:11" ht="30" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B17" s="10">
         <v>256</v>
@@ -10391,9 +10392,9 @@
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="39.75" thickBot="1">
+    <row r="18" spans="1:11" ht="44" thickBot="1">
       <c r="A18" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B18" s="2">
         <f>ROUND(1.1*B17,0)</f>
@@ -10435,8 +10436,8 @@
       <c r="D19" s="2"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="22" spans="1:11" ht="27" thickBot="1">
+    <row r="21" spans="1:11" ht="16" thickBot="1"/>
+    <row r="22" spans="1:11" ht="30" thickBot="1">
       <c r="A22" s="9" t="s">
         <v>85</v>
       </c>
@@ -10451,10 +10452,10 @@
       </c>
       <c r="E22" s="12"/>
       <c r="H22" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="27" thickBot="1">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
@@ -10472,7 +10473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1">
+    <row r="24" spans="1:11" ht="16" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
@@ -10496,9 +10497,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="27" thickBot="1">
+    <row r="25" spans="1:11" ht="30" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B25" s="10">
         <v>351</v>
@@ -10517,9 +10518,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="52.5" thickBot="1">
+    <row r="26" spans="1:11" ht="58" thickBot="1">
       <c r="A26" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B26" s="10">
         <f>ROUND(1.1*B25,0)</f>
@@ -10553,16 +10554,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1">
+    <row r="1" spans="1:10" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -10576,7 +10577,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:10" ht="27" thickBot="1">
+    <row r="2" spans="1:10" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -10597,7 +10598,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1">
+    <row r="3" spans="1:10" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -10618,7 +10619,7 @@
         <v>0.92622883301508352</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="27" thickBot="1">
+    <row r="4" spans="1:10" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -10637,8 +10638,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1">
+    <row r="6" spans="1:10" ht="16" thickBot="1"/>
+    <row r="7" spans="1:10" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -10659,7 +10660,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="27" thickBot="1">
+    <row r="8" spans="1:10" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -10683,7 +10684,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1">
+    <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -10712,7 +10713,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="27" thickBot="1">
+    <row r="10" spans="1:10" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -10752,7 +10753,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1">
+    <row r="13" spans="1:10" ht="16" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -10775,7 +10776,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="27" thickBot="1">
+    <row r="14" spans="1:10" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -10805,7 +10806,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
+    <row r="15" spans="1:10" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -10840,9 +10841,9 @@
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="27" thickBot="1">
+    <row r="16" spans="1:10" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B16" s="10">
         <v>691</v>
@@ -10864,9 +10865,9 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="39.75" thickBot="1">
+    <row r="17" spans="1:10" ht="44" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B17" s="2">
         <f>ROUND(1.1*B16,0)</f>
@@ -10911,8 +10912,8 @@
         <v>219</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1"/>
-    <row r="21" spans="1:10" ht="27" thickBot="1">
+    <row r="20" spans="1:10" ht="16" thickBot="1"/>
+    <row r="21" spans="1:10" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
@@ -10925,7 +10926,7 @@
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
     </row>
-    <row r="22" spans="1:10" ht="27" thickBot="1">
+    <row r="22" spans="1:10" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -10941,7 +10942,7 @@
       </c>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" thickBot="1">
+    <row r="23" spans="1:10" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -10959,9 +10960,9 @@
       </c>
       <c r="E23" s="20"/>
     </row>
-    <row r="24" spans="1:10" ht="27" thickBot="1">
+    <row r="24" spans="1:10" ht="30" thickBot="1">
       <c r="A24" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B24" s="10">
         <v>609</v>
@@ -10975,9 +10976,9 @@
       </c>
       <c r="E24" s="20"/>
     </row>
-    <row r="25" spans="1:10" ht="52.5" thickBot="1">
+    <row r="25" spans="1:10" ht="58" thickBot="1">
       <c r="A25" s="5" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B25" s="10">
         <f>ROUND(1.1*B24,0)</f>
@@ -10993,7 +10994,7 @@
       </c>
       <c r="E25" s="20"/>
       <c r="G25" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -11002,16 +11003,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1">
+    <row r="1" spans="1:13" ht="16" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>14</v>
       </c>
@@ -11025,7 +11026,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:13" ht="27" thickBot="1">
+    <row r="2" spans="1:13" ht="30" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -11046,7 +11047,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1">
+    <row r="3" spans="1:13" ht="16" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
@@ -11067,7 +11068,7 @@
         <v>0.9267197256851698</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="27" thickBot="1">
+    <row r="4" spans="1:13" ht="30" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -11086,8 +11087,8 @@
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
     </row>
-    <row r="6" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:13" ht="15.75" thickBot="1">
+    <row r="6" spans="1:13" ht="16" thickBot="1"/>
+    <row r="7" spans="1:13" ht="16" thickBot="1">
       <c r="A7" s="9" t="s">
         <v>17</v>
       </c>
@@ -11108,7 +11109,7 @@
       </c>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:13" ht="27" thickBot="1">
+    <row r="8" spans="1:13" ht="30" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -11132,7 +11133,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1">
+    <row r="9" spans="1:13" ht="16" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -11161,7 +11162,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="27" thickBot="1">
+    <row r="10" spans="1:13" ht="30" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -11201,7 +11202,7 @@
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="27" thickBot="1">
+    <row r="13" spans="1:13" ht="30" thickBot="1">
       <c r="A13" s="9" t="s">
         <v>13</v>
       </c>
@@ -11230,7 +11231,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="27" thickBot="1">
+    <row r="14" spans="1:13" ht="30" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
@@ -11261,7 +11262,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -11297,9 +11298,9 @@
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="27" thickBot="1">
+    <row r="16" spans="1:13" ht="30" thickBot="1">
       <c r="A16" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B16" s="10">
         <v>454</v>
@@ -11328,9 +11329,9 @@
         <v>233</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="39.75" thickBot="1">
+    <row r="17" spans="1:13" ht="44" thickBot="1">
       <c r="A17" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B17" s="2">
         <f>ROUND(1.1*B16,0)</f>
@@ -11379,8 +11380,8 @@
         <v>235</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" thickBot="1"/>
-    <row r="21" spans="1:13" ht="27" thickBot="1">
+    <row r="20" spans="1:13" ht="16" thickBot="1"/>
+    <row r="21" spans="1:13" ht="30" thickBot="1">
       <c r="A21" s="9" t="s">
         <v>85</v>
       </c>
@@ -11392,10 +11393,10 @@
       </c>
       <c r="D21" s="12"/>
       <c r="G21" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="27" thickBot="1">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="30" thickBot="1">
       <c r="A22" s="5" t="s">
         <v>10</v>
       </c>
@@ -11410,7 +11411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" thickBot="1">
+    <row r="23" spans="1:13" ht="16" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
@@ -11427,7 +11428,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="39.75" thickBot="1">
+    <row r="24" spans="1:13" ht="44" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>89</v>
       </c>
@@ -11452,12 +11453,12 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75" thickBot="1">
+    <row r="29" spans="1:13" ht="16" thickBot="1">
       <c r="A29" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="27" thickBot="1">
+    <row r="30" spans="1:13" ht="30" thickBot="1">
       <c r="A30" s="9" t="s">
         <v>85</v>
       </c>
@@ -11470,7 +11471,7 @@
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:13" ht="27" thickBot="1">
+    <row r="31" spans="1:13" ht="30" thickBot="1">
       <c r="A31" s="5" t="s">
         <v>10</v>
       </c>
@@ -11486,7 +11487,7 @@
       </c>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" thickBot="1">
+    <row r="32" spans="1:13" ht="16" thickBot="1">
       <c r="A32" s="5" t="s">
         <v>11</v>
       </c>
@@ -11504,7 +11505,7 @@
       </c>
       <c r="E32" s="20"/>
     </row>
-    <row r="33" spans="1:5" ht="39.75" thickBot="1">
+    <row r="33" spans="1:5" ht="44" thickBot="1">
       <c r="A33" s="5" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Modify Urban quotas CN
</commit_message>
<xml_diff>
--- a/questionnaires/quotas.xlsx
+++ b/questionnaires/quotas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bluebii/Library/Mobile Documents/com~apple~CloudDocs/TRAVAIL/Jobs/Stantcheva_2020:21/OECD/oecd_climate/questionnaires/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE1C0AE-7F50-0445-A188-53A1729D7F1C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72080CAC-68D6-094D-8A9F-C076A981542A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="15" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" tabRatio="923" firstSheet="12" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quotas_US" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="341">
   <si>
     <t>IDF</t>
   </si>
@@ -1061,6 +1061,30 @@
   </si>
   <si>
     <t>Eastern Anatolia + Southeast Anatolia</t>
+  </si>
+  <si>
+    <t>DEPRECATED</t>
+  </si>
+  <si>
+    <t>&lt;10k</t>
+  </si>
+  <si>
+    <t>urban_category</t>
+  </si>
+  <si>
+    <t>10k-500k</t>
+  </si>
+  <si>
+    <t>&gt;500k</t>
+  </si>
+  <si>
+    <t>https://journals.openedition.org/cybergeo/28554</t>
+  </si>
+  <si>
+    <t>Table 1 (first row) + Total Census population 2010</t>
+  </si>
+  <si>
+    <t>https://journals.openedition.org/cybergeo/docannexe/image/28554/img-6.png</t>
   </si>
 </sst>
 </file>
@@ -1175,7 +1199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1185,6 +1209,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1218,7 +1248,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1291,6 +1321,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4038,10 +4069,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
@@ -4362,174 +4393,277 @@
       <c r="D17" s="2"/>
       <c r="E17" s="11"/>
     </row>
-    <row r="19" spans="1:9" ht="16" thickBot="1">
-      <c r="A19" s="13" t="s">
+    <row r="22" spans="1:9" ht="30" thickBot="1">
+      <c r="A22" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>0.36999306854688396</v>
+      </c>
+      <c r="C23">
+        <v>0.35274265629581675</v>
+      </c>
+      <c r="D23">
+        <v>0.27726427515729923</v>
+      </c>
+      <c r="E23" s="17">
+        <f>SUM(B23:D23)</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="10">
+        <f>ROUND(2000*B23,0)</f>
+        <v>740</v>
+      </c>
+      <c r="C24" s="10">
+        <f>ROUND(2000*C23,0)</f>
+        <v>705</v>
+      </c>
+      <c r="D24" s="10">
+        <f>ROUND(2000*D23,0)</f>
+        <v>555</v>
+      </c>
+      <c r="E24" s="3">
+        <f>SUM(B24:D24)</f>
+        <v>2000</v>
+      </c>
+      <c r="G24" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" thickBot="1">
+      <c r="A25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="2">
+        <f>ROUND(2200*B23,0)</f>
+        <v>814</v>
+      </c>
+      <c r="C25" s="2">
+        <f>ROUND(2200*C23,0)</f>
+        <v>776</v>
+      </c>
+      <c r="D25" s="2">
+        <f>ROUND(2200*D23,0)</f>
+        <v>610</v>
+      </c>
+      <c r="E25" s="3">
+        <f>SUM(B25:D25)</f>
+        <v>2200</v>
+      </c>
+      <c r="H25" t="s">
+        <v>339</v>
+      </c>
+      <c r="I25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="11"/>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="40" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="16" thickBot="1">
+      <c r="A32" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B32" t="s">
         <v>51</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16" thickBot="1">
-      <c r="A20" s="5" t="s">
+    <row r="33" spans="1:9" ht="16" thickBot="1">
+      <c r="A33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B20">
+      <c r="B33">
         <v>0.4437874</v>
       </c>
-      <c r="C20">
+      <c r="C33">
         <v>0.55621259999999995</v>
       </c>
-      <c r="D20" s="17">
-        <f>SUM(B20:C20)</f>
+      <c r="D33" s="17">
+        <f>SUM(B33:C33)</f>
         <v>1</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F33" t="s">
         <v>186</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G33" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="16" thickBot="1">
-      <c r="A21" s="5" t="s">
+    <row r="34" spans="1:9" ht="16" thickBot="1">
+      <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B21">
-        <f>ROUND(2000*B20,0)</f>
+      <c r="B34">
+        <f>ROUND(2000*B33,0)</f>
         <v>888</v>
       </c>
-      <c r="C21">
-        <f>ROUND(2000*C20,0)</f>
+      <c r="C34">
+        <f>ROUND(2000*C33,0)</f>
         <v>1112</v>
       </c>
-      <c r="D21">
-        <f>SUM(B21:C21)</f>
+      <c r="D34">
+        <f>SUM(B34:C34)</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="30" thickBot="1">
-      <c r="A22" s="5" t="s">
+    <row r="35" spans="1:9" ht="30" thickBot="1">
+      <c r="A35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B22">
-        <f>ROUND(2200*B20,0)</f>
+      <c r="B35">
+        <f>ROUND(2200*B33,0)</f>
         <v>976</v>
       </c>
-      <c r="C22">
-        <f>ROUND(2200*C20,0)</f>
+      <c r="C35">
+        <f>ROUND(2200*C33,0)</f>
         <v>1224</v>
       </c>
-      <c r="D22">
-        <f>SUM(B22:C22)</f>
+      <c r="D35">
+        <f>SUM(B35:C35)</f>
         <v>2200</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G35" t="s">
         <v>189</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H35" t="s">
         <v>190</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I35" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="9" t="s">
+    <row r="36" spans="1:9">
+      <c r="A36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="30" t="s">
+      <c r="G36" s="30" t="s">
         <v>191</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="H36" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="I23">
+      <c r="I36">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
-      <c r="G24" s="30" t="s">
+    <row r="37" spans="1:9">
+      <c r="G37" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="H24" s="30" t="s">
+      <c r="H37" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="I24">
+      <c r="I37">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
-      <c r="G25" s="30" t="s">
+    <row r="38" spans="1:9">
+      <c r="G38" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="H38" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="I25">
+      <c r="I38">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
-      <c r="G26" t="s">
+    <row r="39" spans="1:9">
+      <c r="G39" t="s">
         <v>196</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H39" t="s">
         <v>197</v>
       </c>
-      <c r="I26">
+      <c r="I39">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
-      <c r="G27" t="s">
+    <row r="40" spans="1:9">
+      <c r="G40" t="s">
         <v>198</v>
       </c>
-      <c r="I27">
+      <c r="I40">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
-      <c r="G28" t="s">
+    <row r="41" spans="1:9">
+      <c r="G41" t="s">
         <v>199</v>
       </c>
-      <c r="I28">
+      <c r="I41">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="G29" t="s">
+    <row r="42" spans="1:9">
+      <c r="G42" t="s">
         <v>200</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H42" t="s">
         <v>201</v>
       </c>
-      <c r="I29">
+      <c r="I42">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
-      <c r="G30" t="s">
+    <row r="43" spans="1:9">
+      <c r="G43" t="s">
         <v>202</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H43" t="s">
         <v>203</v>
       </c>
-      <c r="I30">
+      <c r="I43">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="G31" t="s">
+    <row r="44" spans="1:9">
+      <c r="G44" t="s">
         <v>204</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H44" t="s">
         <v>205</v>
       </c>
-      <c r="I31">
+      <c r="I44">
         <v>0</v>
       </c>
     </row>
@@ -6062,11 +6196,11 @@
         <v>0.25032612031513901</v>
       </c>
       <c r="F15" s="17">
-        <f>SUM(A15:E15)</f>
+        <f t="shared" ref="F15:G17" si="2">SUM(A15:E15)</f>
         <v>1</v>
       </c>
       <c r="G15" s="17">
-        <f>SUM(B15:F15)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I15" t="s">
@@ -6097,11 +6231,11 @@
         <v>501</v>
       </c>
       <c r="F16" s="3">
-        <f>SUM(A16:E16)</f>
+        <f t="shared" si="2"/>
         <v>2001</v>
       </c>
       <c r="G16" s="3">
-        <f>SUM(B16:F16)</f>
+        <f t="shared" si="2"/>
         <v>4002</v>
       </c>
       <c r="I16" t="s">
@@ -6132,11 +6266,11 @@
         <v>551</v>
       </c>
       <c r="F17" s="3">
-        <f>SUM(A17:E17)</f>
+        <f t="shared" si="2"/>
         <v>2201</v>
       </c>
       <c r="G17" s="3">
-        <f>SUM(B17:F17)</f>
+        <f t="shared" si="2"/>
         <v>4402</v>
       </c>
       <c r="I17" t="s">
@@ -6292,7 +6426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>

</xml_diff>